<commit_message>
oracle now support xls inserting
</commit_message>
<xml_diff>
--- a/test/schema/oracle/gameAdmin1.xlsx
+++ b/test/schema/oracle/gameAdmin1.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="1120" windowWidth="24480" windowHeight="14940" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1600" yWindow="760" windowWidth="24480" windowHeight="14940" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Domain" sheetId="1" r:id="rId1"/>
     <sheet name="T_MON_SERVICE" sheetId="2" r:id="rId2"/>
+    <sheet name="Scene" sheetId="3" r:id="rId3"/>
+    <sheet name="Area" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,8 +21,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>作者</author>
+  </authors>
+  <commentList>
+    <comment ref="F7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+进入关卡时，玩家所在的第一个区域</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="86">
   <si>
     <t>mon</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -186,19 +224,157 @@
   </si>
   <si>
     <t>DATE</t>
+  </si>
+  <si>
+    <t>Scene</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>SceneID</t>
+  </si>
+  <si>
+    <t>SceneName</t>
+  </si>
+  <si>
+    <t>SceneType</t>
+  </si>
+  <si>
+    <t>AreaID</t>
+  </si>
+  <si>
+    <t>InitialArea</t>
+  </si>
+  <si>
+    <t>VisiableInStage1</t>
+  </si>
+  <si>
+    <t>AreaX</t>
+  </si>
+  <si>
+    <t>AreaY</t>
+  </si>
+  <si>
+    <t>AreaZ</t>
+  </si>
+  <si>
+    <t>NUMBER(10, 2)</t>
+  </si>
+  <si>
+    <t>Index</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>场景ID</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>场景名称</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>场景种类（1为主城，2为野外，3为关卡）</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>区域ID</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否是关卡初始区域</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>1阶段能否看到</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>区域在场景中位置X</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>区域在场景中位置Y</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>区域在场景中位置Z</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>场景资源</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>出生点X</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>出生点Y</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>出生点Z</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>刷怪表路径</t>
+  </si>
+  <si>
+    <t>背景音乐</t>
+  </si>
+  <si>
+    <t>boss音乐</t>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>SceneResource</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>BornPosition_X</t>
+  </si>
+  <si>
+    <t>BornPosition_Y</t>
+  </si>
+  <si>
+    <t>BornPosition_Z</t>
+  </si>
+  <si>
+    <t>BornFaceTo</t>
+  </si>
+  <si>
+    <t>NpcWavePath</t>
+  </si>
+  <si>
+    <t>BackgoundMusic</t>
+  </si>
+  <si>
+    <t>BossMusic</t>
+  </si>
+  <si>
+    <t>mon</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>VARCHAR2(128)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -247,8 +423,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -258,6 +457,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -286,13 +491,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -313,11 +532,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="11" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="11" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="16">
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="표준 5" xfId="3"/>
+    <cellStyle name="常规 2" xfId="11"/>
     <cellStyle name="普通 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -647,10 +890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -697,10 +940,44 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
+    <row r="3" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" location="T_MON_SERVICE!A1" display="T_MON_SERVICE"/>
+    <hyperlink ref="C3" location="Scene!A1" display="Scene"/>
+    <hyperlink ref="C4" location="Area!A1" display="Area"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -715,9 +992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -928,4 +1203,396 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
detect xls change and sync to db
</commit_message>
<xml_diff>
--- a/test/schema/oracle/gameAdmin1.xlsx
+++ b/test/schema/oracle/gameAdmin1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="760" windowWidth="24480" windowHeight="14940" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="1600" yWindow="760" windowWidth="24480" windowHeight="14940" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Domain" sheetId="1" r:id="rId1"/>
@@ -217,9 +217,6 @@
     <t>NUMBER(4,0)</t>
   </si>
   <si>
-    <t>FLOAT (24)</t>
-  </si>
-  <si>
     <t>NUMBER(19, 0)</t>
   </si>
   <si>
@@ -363,6 +360,9 @@
   </si>
   <si>
     <t>VARCHAR2(128)</t>
+  </si>
+  <si>
+    <t>FLOAT(24)</t>
   </si>
 </sst>
 </file>
@@ -945,10 +945,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -958,13 +958,13 @@
     </row>
     <row r="4" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1">
       <c r="A4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="C4" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -992,7 +992,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -1111,7 +1113,7 @@
         <v>28</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>29</v>
@@ -1127,7 +1129,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>23</v>
@@ -1143,7 +1145,7 @@
         <v>33</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>34</v>
@@ -1159,7 +1161,7 @@
         <v>36</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>23</v>
@@ -1175,7 +1177,7 @@
         <v>37</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>18</v>
@@ -1209,7 +1211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -1237,7 +1239,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>38</v>
@@ -1250,12 +1252,12 @@
       </c>
       <c r="E2" s="7"/>
       <c r="F2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>38</v>
@@ -1266,15 +1268,15 @@
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>18</v>
@@ -1282,12 +1284,12 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>38</v>
@@ -1298,12 +1300,12 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>38</v>
@@ -1314,12 +1316,12 @@
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>38</v>
@@ -1330,12 +1332,12 @@
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>38</v>
@@ -1346,15 +1348,15 @@
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>18</v>
@@ -1362,15 +1364,15 @@
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>18</v>
@@ -1378,15 +1380,15 @@
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>56</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>18</v>
@@ -1394,7 +1396,7 @@
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1443,7 +1445,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>38</v>
@@ -1456,15 +1458,15 @@
       </c>
       <c r="E2" s="7"/>
       <c r="F2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>18</v>
@@ -1472,15 +1474,15 @@
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>18</v>
@@ -1488,15 +1490,15 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>18</v>
@@ -1504,15 +1506,15 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>18</v>
@@ -1520,12 +1522,12 @@
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>38</v>
@@ -1536,12 +1538,12 @@
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>40</v>
@@ -1552,12 +1554,12 @@
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>40</v>
@@ -1568,12 +1570,12 @@
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>40</v>
@@ -1584,7 +1586,7 @@
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>